<commit_message>
Inserting/Deleting rows/columns now shift the named ranges too.
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/ShiftingFormulas.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/ShiftingFormulas.xlsx
@@ -10,8 +10,8 @@
     <x:sheet name="WS2" sheetId="3" r:id="rId3"/>
   </x:sheets>
   <x:definedNames>
-    <x:definedName name="WorksheetB4C4" localSheetId="0">'Shifting Formulas'!$B$4:$C$4</x:definedName>
-    <x:definedName name="WorkbookB4C4">'Shifting Formulas'!$B$4:$C$4</x:definedName>
+    <x:definedName name="WorksheetB4C4" localSheetId="0">'Shifting Formulas'!$C$5:$D$5</x:definedName>
+    <x:definedName name="WorkbookB4C4">'Shifting Formulas'!$C$5:$D$5</x:definedName>
   </x:definedNames>
   <x:calcPr calcId="125725"/>
 </x:workbook>

</xml_diff>